<commit_message>
add new code for multiple test data like one data rone then second data row
</commit_message>
<xml_diff>
--- a/DataSheet/FOS3.xlsx
+++ b/DataSheet/FOS3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55E80B7-D395-4BBE-AF24-7FB2277E32B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22F18E3-C005-4CF4-8D14-529D288DF531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="187">
   <si>
     <t>Si_No</t>
   </si>
@@ -247,9 +247,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>START_APPLICATION</t>
   </si>
   <si>
@@ -545,13 +542,119 @@
   </si>
   <si>
     <t>37</t>
+  </si>
+  <si>
+    <t>ScrollUsingCoordinate</t>
+  </si>
+  <si>
+    <t>(//*[@class='android.widget.CheckBox'])[2]</t>
+  </si>
+  <si>
+    <t>(//android.view.View[@content-desc="PAN Verification"])[2]</t>
+  </si>
+  <si>
+    <r>
+      <t>(//android.view.View[@content-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>="Proof Of Identity"])[2]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@content-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>="</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Aadhaar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Card(Preferred)"]/android.view.View</t>
+    </r>
+  </si>
+  <si>
+    <t>ScrollIntoElement</t>
+  </si>
+  <si>
+    <t>POI_ScrollTo_DL</t>
+  </si>
+  <si>
+    <t>Driving License</t>
+  </si>
+  <si>
+    <t>WAIT(4000)</t>
+  </si>
+  <si>
+    <t>CoordinateScrollforPanForm60</t>
+  </si>
+  <si>
+    <t>CoordinateScrollForm60ToPAN</t>
+  </si>
+  <si>
+    <t>WAIT(9000)</t>
+  </si>
+  <si>
+    <t>//android.view.View[@content-desc="Driving License"]</t>
+  </si>
+  <si>
+    <t>500.1943.547.950</t>
+  </si>
+  <si>
+    <t>487.783.390.1893</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,8 +687,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F7F5F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF3F7F5F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,25 +710,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,20 +736,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A38"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,13 +1156,13 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -1087,19 +1185,19 @@
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L3" t="s">
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N3" t="s">
         <v>25</v>
@@ -1122,25 +1220,25 @@
         <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L4" t="s">
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N4" t="s">
         <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1160,31 +1258,31 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N5" t="s">
         <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1210,13 +1308,13 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L6" t="s">
         <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N6" t="s">
         <v>28</v>
@@ -1248,13 +1346,13 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N7" t="s">
         <v>60</v>
@@ -1286,13 +1384,13 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N8" t="s">
         <v>61</v>
@@ -1324,13 +1422,13 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L9" t="s">
         <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N9" t="s">
         <v>62</v>
@@ -1360,16 +1458,16 @@
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L10" t="s">
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O10" t="s">
         <v>63</v>
@@ -1383,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -1398,25 +1496,25 @@
         <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L11" t="s">
         <v>67</v>
       </c>
       <c r="M11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N11" t="s">
         <v>68</v>
       </c>
       <c r="O11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1427,7 +1525,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -1448,13 +1546,13 @@
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L12" t="s">
         <v>67</v>
       </c>
       <c r="M12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N12" t="s">
         <v>69</v>
@@ -1471,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1483,13 +1581,13 @@
         <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L13" t="s">
         <v>67</v>
       </c>
       <c r="M13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N13" t="s">
         <v>70</v>
@@ -1506,40 +1604,40 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
       </c>
       <c r="K14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" t="s">
         <v>111</v>
       </c>
-      <c r="L14" t="s">
-        <v>112</v>
-      </c>
       <c r="M14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1550,16 +1648,16 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
         <v>29</v>
@@ -1571,16 +1669,16 @@
         <v>17</v>
       </c>
       <c r="K15" t="s">
+        <v>110</v>
+      </c>
+      <c r="L15" t="s">
         <v>111</v>
       </c>
-      <c r="L15" t="s">
-        <v>112</v>
-      </c>
       <c r="M15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O15" t="s">
         <v>66</v>
@@ -1594,7 +1692,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1606,16 +1704,16 @@
         <v>17</v>
       </c>
       <c r="K16" t="s">
+        <v>110</v>
+      </c>
+      <c r="L16" t="s">
         <v>111</v>
       </c>
-      <c r="L16" t="s">
-        <v>112</v>
-      </c>
       <c r="M16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O16" t="s">
         <v>58</v>
@@ -1623,13 +1721,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
@@ -1638,42 +1736,42 @@
         <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
         <v>17</v>
       </c>
       <c r="K17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" t="s">
         <v>111</v>
       </c>
-      <c r="L17" t="s">
-        <v>112</v>
-      </c>
       <c r="M17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
@@ -1682,7 +1780,7 @@
         <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
         <v>29</v>
@@ -1694,30 +1792,30 @@
         <v>17</v>
       </c>
       <c r="K18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L18" t="s">
         <v>111</v>
       </c>
-      <c r="L18" t="s">
-        <v>112</v>
-      </c>
       <c r="M18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
@@ -1726,42 +1824,42 @@
         <v>39</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
         <v>30</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J19" t="s">
         <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1770,7 +1868,7 @@
         <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G20" t="s">
         <v>29</v>
@@ -1782,30 +1880,30 @@
         <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
@@ -1813,43 +1911,43 @@
       <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>83</v>
+      <c r="F21" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="G21" t="s">
         <v>30</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1857,8 +1955,8 @@
       <c r="E22" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>83</v>
+      <c r="F22" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="G22" t="s">
         <v>29</v>
@@ -1870,30 +1968,30 @@
         <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
@@ -1901,8 +1999,8 @@
       <c r="E23" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>84</v>
+      <c r="F23" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="G23" t="s">
         <v>29</v>
@@ -1914,30 +2012,30 @@
         <v>17</v>
       </c>
       <c r="K23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -1945,43 +2043,43 @@
       <c r="E24" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>85</v>
+      <c r="F24" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="G24" t="s">
         <v>30</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J24" t="s">
         <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
@@ -1989,8 +2087,8 @@
       <c r="E25" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>85</v>
+      <c r="F25" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="G25" t="s">
         <v>29</v>
@@ -2002,65 +2100,65 @@
         <v>17</v>
       </c>
       <c r="K25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J26" t="s">
         <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -2068,43 +2166,43 @@
       <c r="E27" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>86</v>
+      <c r="F27" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J27" t="s">
         <v>17</v>
       </c>
       <c r="K27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
@@ -2112,8 +2210,8 @@
       <c r="E28" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>86</v>
+      <c r="F28" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="G28" t="s">
         <v>29</v>
@@ -2125,30 +2223,30 @@
         <v>17</v>
       </c>
       <c r="K28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
@@ -2157,7 +2255,7 @@
         <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G29" t="s">
         <v>29</v>
@@ -2169,30 +2267,30 @@
         <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
@@ -2201,42 +2299,42 @@
         <v>39</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G30" t="s">
         <v>30</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J30" t="s">
         <v>17</v>
       </c>
       <c r="K30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
@@ -2245,7 +2343,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G31" t="s">
         <v>29</v>
@@ -2257,30 +2355,30 @@
         <v>17</v>
       </c>
       <c r="K31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
@@ -2289,42 +2387,42 @@
         <v>39</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G32" t="s">
         <v>30</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J32" t="s">
         <v>17</v>
       </c>
       <c r="K32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
@@ -2333,7 +2431,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" t="s">
         <v>29</v>
@@ -2345,30 +2443,30 @@
         <v>17</v>
       </c>
       <c r="K33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
@@ -2377,51 +2475,51 @@
         <v>39</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G34" t="s">
         <v>30</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" t="s">
         <v>17</v>
       </c>
       <c r="K34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
       </c>
       <c r="E35" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G35" t="s">
         <v>29</v>
@@ -2433,83 +2531,83 @@
         <v>17</v>
       </c>
       <c r="K35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
       </c>
       <c r="E36" t="s">
         <v>39</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G36" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J36" t="s">
         <v>17</v>
       </c>
       <c r="K36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
       </c>
       <c r="E37" t="s">
         <v>39</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G37" t="s">
         <v>29</v>
@@ -2521,58 +2619,532 @@
         <v>17</v>
       </c>
       <c r="K37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" t="s">
+        <v>110</v>
+      </c>
+      <c r="L38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M38" t="s">
+        <v>120</v>
+      </c>
+      <c r="N38" t="s">
+        <v>70</v>
+      </c>
+      <c r="O38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" t="s">
+        <v>181</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="J39" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" t="s">
+        <v>110</v>
+      </c>
+      <c r="L39" t="s">
+        <v>112</v>
+      </c>
+      <c r="M39" t="s">
+        <v>122</v>
+      </c>
+      <c r="N39" t="s">
+        <v>142</v>
+      </c>
+      <c r="O39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" t="s">
+        <v>110</v>
+      </c>
+      <c r="L40" t="s">
+        <v>112</v>
+      </c>
+      <c r="M40" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" t="s">
+        <v>142</v>
+      </c>
+      <c r="O40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" t="s">
+        <v>67</v>
+      </c>
+      <c r="M41" t="s">
+        <v>120</v>
+      </c>
+      <c r="N41" t="s">
+        <v>70</v>
+      </c>
+      <c r="O41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" t="s">
+        <v>182</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" t="s">
+        <v>110</v>
+      </c>
+      <c r="L42" t="s">
+        <v>112</v>
+      </c>
+      <c r="M42" t="s">
+        <v>122</v>
+      </c>
+      <c r="N42" t="s">
+        <v>142</v>
+      </c>
+      <c r="O42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" t="s">
+        <v>110</v>
+      </c>
+      <c r="L43" t="s">
+        <v>112</v>
+      </c>
+      <c r="M43" t="s">
+        <v>122</v>
+      </c>
+      <c r="N43" t="s">
+        <v>142</v>
+      </c>
+      <c r="O43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J44" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" t="s">
+        <v>110</v>
+      </c>
+      <c r="L44" t="s">
+        <v>112</v>
+      </c>
+      <c r="M44" t="s">
+        <v>122</v>
+      </c>
+      <c r="N44" t="s">
+        <v>142</v>
+      </c>
+      <c r="O44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J45" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" t="s">
+        <v>110</v>
+      </c>
+      <c r="L45" t="s">
+        <v>112</v>
+      </c>
+      <c r="M45" t="s">
+        <v>122</v>
+      </c>
+      <c r="N45" t="s">
+        <v>142</v>
+      </c>
+      <c r="O45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" t="s">
+        <v>178</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" t="s">
+        <v>110</v>
+      </c>
+      <c r="L46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M46" t="s">
+        <v>122</v>
+      </c>
+      <c r="N46" t="s">
+        <v>142</v>
+      </c>
+      <c r="O46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" t="s">
+        <v>110</v>
+      </c>
+      <c r="L47" t="s">
+        <v>67</v>
+      </c>
+      <c r="M47" t="s">
+        <v>120</v>
+      </c>
+      <c r="N47" t="s">
+        <v>70</v>
+      </c>
+      <c r="O47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" t="s">
+        <v>110</v>
+      </c>
+      <c r="L48" t="s">
+        <v>112</v>
+      </c>
+      <c r="M48" t="s">
+        <v>122</v>
+      </c>
+      <c r="N48" t="s">
+        <v>142</v>
+      </c>
+      <c r="O48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J49" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" t="s">
+        <v>110</v>
+      </c>
+      <c r="L49" t="s">
+        <v>67</v>
+      </c>
+      <c r="M49" t="s">
+        <v>120</v>
+      </c>
+      <c r="N49" t="s">
+        <v>70</v>
+      </c>
+      <c r="O49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" t="s">
-        <v>111</v>
-      </c>
-      <c r="L38" t="s">
-        <v>113</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="J50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" t="s">
+        <v>110</v>
+      </c>
+      <c r="L50" t="s">
+        <v>112</v>
+      </c>
+      <c r="M50" t="s">
         <v>65</v>
       </c>
-      <c r="N38" t="s">
-        <v>144</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="N50" t="s">
+        <v>143</v>
+      </c>
+      <c r="O50" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F42" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2582,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2595,9 +3167,12 @@
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2625,8 +3200,17 @@
       <c r="I1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2643,16 +3227,63 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>8</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="K2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="K3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>